<commit_message>
Måle resultater af enhedstest og rettelser komponentværdier
Le Golden Doc for Sara
</commit_message>
<xml_diff>
--- a/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
+++ b/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ark3" sheetId="3" r:id="rId1"/>
     <sheet name="Filter" sheetId="4" r:id="rId2"/>
-    <sheet name="Forstærker" sheetId="1" r:id="rId3"/>
+    <sheet name="Filter og forstærker sammen" sheetId="5" r:id="rId3"/>
+    <sheet name="Forstærker" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Forstærkning</t>
   </si>
@@ -146,6 +147,12 @@
   </si>
   <si>
     <t>Amplitude ud i V</t>
+  </si>
+  <si>
+    <t>For meget offset!</t>
+  </si>
+  <si>
+    <t>Fasedrej</t>
   </si>
 </sst>
 </file>
@@ -287,6 +294,1168 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dæmpning</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> af signal ved forskellige frekvenser</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Filter!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Filter!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Filter!$C$3:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.75E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="461467712"/>
+        <c:axId val="461467320"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Filter!$A$5:$A$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="18"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>150</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Filter!$C$5:$C$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="18"/>
+                      <c:pt idx="0">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.4700000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.36</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2.27</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2.14</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.04</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.97</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.81</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.72</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.61</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.48</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1.18</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.96</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.77</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.64</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.55000000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.46</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.28999999999999998</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="461467712"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="461467320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="461467320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="461467712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Filter!$A$27:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Filter!$C$27:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.9588001734407516</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8539390651933152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4582400594021312</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1205171438624548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6082754669838177</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1926033485179754</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8893245232318581</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1535714973836901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.7105689381509777</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1365175206369944</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4052343078991476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4376401461225072</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.35457533920863205</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.2701854965503623</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.8764005203222562</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-5.1927462101151223</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6.7448433663685181</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-10.752040042020878</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="413072904"/>
+        <c:axId val="413074472"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Filter!$A$27:$A$44</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="18"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>150</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="413072904"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413074472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="413074472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413072904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="da-DK"/>
               <a:t>DC-forstærkning</a:t>
             </a:r>
@@ -384,8 +1553,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.4595733838928577E-4"/>
-                  <c:y val="0.37254648060469814"/>
+                  <c:x val="-4.453472989021557E-2"/>
+                  <c:y val="0.39117961379776778"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -407,17 +1576,17 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1300" b="1" baseline="0"/>
-                      <a:t>y = 663,38x - 0,6127</a:t>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 386,38x + 0,5547</a:t>
                     </a:r>
                     <a:br>
-                      <a:rPr lang="en-US" sz="1300" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
                     </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1300" b="1" baseline="0"/>
-                      <a:t>R² = 0,9864</a:t>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0,9979</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="1300" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -453,54 +1622,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Forstærker!$C$4:$C$9</c:f>
+              <c:f>Forstærker!$C$6:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.6000000000000001E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8999999999999998E-3</c:v>
+                  <c:v>1.9499999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6000000000000003E-3</c:v>
+                  <c:v>3.2500000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9500000000000004E-3</c:v>
+                  <c:v>3.9500000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2000000000000006E-3</c:v>
+                  <c:v>5.5500000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9000000000000008E-3</c:v>
+                  <c:v>6.2000000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2500000000000004E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Forstærker!$D$4:$D$9</c:f>
+              <c:f>Forstærker!$D$6:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.34</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.72</c:v>
+                  <c:v>1.88</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.57</c:v>
+                  <c:v>2.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2.66</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8</c:v>
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -515,11 +1696,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="382446944"/>
-        <c:axId val="382446552"/>
+        <c:axId val="409610112"/>
+        <c:axId val="409612072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="382446944"/>
+        <c:axId val="409610112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,12 +1757,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382446552"/>
+        <c:crossAx val="409612072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="382446552"/>
+        <c:axId val="409612072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +1819,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382446944"/>
+        <c:crossAx val="409610112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -687,7 +1868,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
@@ -828,13 +2009,27 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.5493919661426319E-2"/>
-                  <c:y val="0.40732182616207024"/>
+                  <c:x val="6.3588625816236644E-2"/>
+                  <c:y val="0.32359767201056877"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -856,17 +2051,17 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
-                      <a:t>y = 625,31x + 0,0298</a:t>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 415,76x - 0,0937</a:t>
                     </a:r>
                     <a:br>
-                      <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
                     </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
-                      <a:t>R² = 0,9995</a:t>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0,9993</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -902,54 +2097,78 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Forstærker!$C$20:$C$25</c:f>
+              <c:f>Forstærker!$C$20:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.1000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9750000000000002E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0249999999999999E-3</c:v>
+                  <c:v>3.0499999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1250000000000002E-3</c:v>
+                  <c:v>3.9249999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0499999999999998E-3</c:v>
+                  <c:v>5.0999999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>6.0999999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9500000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8000000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.75E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Forstærker!$D$20:$D$25</c:f>
+              <c:f>Forstærker!$D$20:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.66</c:v>
+                  <c:v>0.38500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.29</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9</c:v>
+                  <c:v>1.1599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.57</c:v>
+                  <c:v>1.5449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2</c:v>
+                  <c:v>1.9850000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8</c:v>
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -964,11 +2183,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="382449296"/>
-        <c:axId val="382446160"/>
+        <c:axId val="409610504"/>
+        <c:axId val="409614424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="382449296"/>
+        <c:axId val="409610504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,12 +2244,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382446160"/>
+        <c:crossAx val="409614424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="382446160"/>
+        <c:axId val="409614424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,7 +2306,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382449296"/>
+        <c:crossAx val="409610504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1216,6 +2435,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2248,7 +3547,1104 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2885,10 +5281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,7 +5294,7 @@
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -2911,277 +5307,597 @@
       <c r="D2" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="C3">
+        <v>2.5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="C4">
+        <v>2.5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>3.8</v>
-      </c>
-      <c r="C3">
-        <f>6.64/2</f>
-        <v>3.32</v>
-      </c>
-      <c r="D3">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B5">
+        <v>2.5</v>
+      </c>
+      <c r="C5">
+        <v>2.5</v>
+      </c>
+      <c r="D5">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>20</v>
       </c>
-      <c r="B4">
-        <v>3.8</v>
-      </c>
-      <c r="C4">
-        <f>6.2/2</f>
-        <v>3.1</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <f>4.94/2</f>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D6">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>30</v>
       </c>
-      <c r="B5">
-        <f>7.6/2</f>
-        <v>3.8</v>
-      </c>
-      <c r="C5">
-        <f>5.6/2</f>
-        <v>2.8</v>
-      </c>
-      <c r="D5">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B7">
+        <v>2.5</v>
+      </c>
+      <c r="C7">
+        <f>4.72/2</f>
+        <v>2.36</v>
+      </c>
+      <c r="D7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>35</v>
       </c>
-      <c r="B6">
-        <f>7.6/2</f>
-        <v>3.8</v>
-      </c>
-      <c r="C6">
-        <f>5.16/2</f>
-        <v>2.58</v>
-      </c>
-      <c r="D6">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B8">
+        <v>2.5</v>
+      </c>
+      <c r="C8">
+        <f>4.54/2</f>
+        <v>2.27</v>
+      </c>
+      <c r="D8">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>40</v>
       </c>
-      <c r="B7">
-        <f t="shared" ref="B7:B15" si="0">7.6/2</f>
-        <v>3.8</v>
-      </c>
-      <c r="C7">
-        <f>4.68/2</f>
-        <v>2.34</v>
-      </c>
-      <c r="D7">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B9">
+        <v>2.5</v>
+      </c>
+      <c r="C9">
+        <f>4.28/2</f>
+        <v>2.14</v>
+      </c>
+      <c r="D9">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>43</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="C8">
-        <f>4.42/2</f>
-        <v>2.21</v>
-      </c>
-      <c r="D8">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>46</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="C9">
-        <f>4.16/2</f>
-        <v>2.08</v>
-      </c>
-      <c r="D9">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>50</v>
-      </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="C10">
-        <f>3.86/2</f>
-        <v>1.93</v>
+        <f>4.08/2</f>
+        <v>2.04</v>
       </c>
       <c r="D10">
         <v>4.8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="C11">
-        <f>3.64/2</f>
-        <v>1.82</v>
+        <f>3.94/2</f>
+        <v>1.97</v>
       </c>
       <c r="D11">
         <v>4.8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>2.5</v>
+      </c>
+      <c r="C12">
+        <f>3.62/2</f>
+        <v>1.81</v>
+      </c>
+      <c r="D12">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>2.5</v>
+      </c>
+      <c r="C13">
+        <f>3.44/2</f>
+        <v>1.72</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>56</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="C12">
-        <f>3.46/2</f>
-        <v>1.73</v>
-      </c>
-      <c r="D12">
-        <v>4.6500000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B14">
+        <v>2.5</v>
+      </c>
+      <c r="C14">
+        <f>3.22/2</f>
+        <v>1.61</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>60</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="C13">
-        <f>3.18/2</f>
-        <v>1.59</v>
-      </c>
-      <c r="D13">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B15">
+        <v>2.5</v>
+      </c>
+      <c r="C15">
+        <f>2.96/2</f>
+        <v>1.48</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>70</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="C14">
-        <f>2.66/2</f>
-        <v>1.33</v>
-      </c>
-      <c r="D14">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>80</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="C15">
-        <f>2.18/2</f>
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D15">
-        <v>3.95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>90</v>
-      </c>
       <c r="B16">
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="C16">
-        <f>1.82/2</f>
-        <v>0.91</v>
+        <f>2.36/2</f>
+        <v>1.18</v>
       </c>
       <c r="D16">
-        <v>3.6</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B17">
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="C17">
-        <f>1.56/2</f>
-        <v>0.78</v>
+        <f>1.92/2</f>
+        <v>0.96</v>
       </c>
       <c r="D17">
-        <v>3.45</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>2.5</v>
+      </c>
+      <c r="C18">
+        <f>1.54/2</f>
+        <v>0.77</v>
+      </c>
+      <c r="D18">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>100</v>
+      </c>
+      <c r="B19">
+        <v>2.5</v>
+      </c>
+      <c r="C19">
+        <f>1.28/2</f>
+        <v>0.64</v>
+      </c>
+      <c r="D19">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>110</v>
       </c>
-      <c r="B18">
-        <v>3.8</v>
-      </c>
-      <c r="C18">
-        <f>1.36/2</f>
-        <v>0.68</v>
-      </c>
-      <c r="D18">
-        <v>3.1</v>
+      <c r="B20">
+        <v>2.5</v>
+      </c>
+      <c r="C20">
+        <f>1.1/2</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D20">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>120</v>
+      </c>
+      <c r="B21">
+        <v>2.5</v>
+      </c>
+      <c r="C21">
+        <f>(920*10^-3)/2</f>
+        <v>0.46</v>
+      </c>
+      <c r="D21">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>150</v>
+      </c>
+      <c r="B22">
+        <v>2.5</v>
+      </c>
+      <c r="C22">
+        <f>(580*10^-3)/2</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D22">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>500</v>
+      </c>
+      <c r="B23">
+        <v>2.5</v>
+      </c>
+      <c r="C23">
+        <f>(55*10^-3)/2</f>
+        <v>2.75E-2</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>2.5</v>
+      </c>
+      <c r="C27">
+        <f>20*LOG10(B27)</f>
+        <v>7.9588001734407516</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <f>4.94/2</f>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:C44" si="0">20*LOG10(B28)</f>
+        <v>7.8539390651933152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <f>4.72/2</f>
+        <v>2.36</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>7.4582400594021312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <f>4.54/2</f>
+        <v>2.27</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>7.1205171438624548</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <f>4.28/2</f>
+        <v>2.14</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>6.6082754669838177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <f>4.08/2</f>
+        <v>2.04</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>6.1926033485179754</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <f>3.94/2</f>
+        <v>1.97</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>5.8893245232318581</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>50</v>
+      </c>
+      <c r="B34">
+        <f>3.62/2</f>
+        <v>1.81</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>5.1535714973836901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <f>3.44/2</f>
+        <v>1.72</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>4.7105689381509777</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>56</v>
+      </c>
+      <c r="B36">
+        <f>3.22/2</f>
+        <v>1.61</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>4.1365175206369944</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>60</v>
+      </c>
+      <c r="B37">
+        <f>2.96/2</f>
+        <v>1.48</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>3.4052343078991476</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>70</v>
+      </c>
+      <c r="B38">
+        <f>2.36/2</f>
+        <v>1.18</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1.4376401461225072</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>80</v>
+      </c>
+      <c r="B39">
+        <f>1.92/2</f>
+        <v>0.96</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>-0.35457533920863205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>90</v>
+      </c>
+      <c r="B40">
+        <f>1.54/2</f>
+        <v>0.77</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>-2.2701854965503623</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>100</v>
+      </c>
+      <c r="B41">
+        <f>1.28/2</f>
+        <v>0.64</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>-3.8764005203222562</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>110</v>
+      </c>
+      <c r="B42">
+        <f>1.1/2</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>-5.1927462101151223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>120</v>
+      </c>
+      <c r="B43">
+        <f>(920*10^-3)/2</f>
+        <v>0.46</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>-6.7448433663685181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>150</v>
+      </c>
+      <c r="B44">
+        <f>(580*10^-3)/2</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>-10.752040042020878</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E25"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
@@ -3216,17 +5932,8 @@
         <f>1*10^-3</f>
         <v>1E-3</v>
       </c>
-      <c r="C4">
-        <f>1.6*10^-3</f>
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D4">
-        <f>580*10^-3</f>
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E9" si="0">D4/C4</f>
-        <v>362.49999999999994</v>
+      <c r="C4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3237,16 +5944,8 @@
         <f>2*10^-3</f>
         <v>2E-3</v>
       </c>
-      <c r="C5">
-        <f>2.9*10^-3</f>
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="D5">
-        <v>1.34</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>462.06896551724145</v>
+      <c r="C5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,15 +5957,16 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C6">
-        <f>3.6*10^-3</f>
-        <v>3.6000000000000003E-3</v>
+        <f>1.25*10^-3</f>
+        <v>1.25E-3</v>
       </c>
       <c r="D6">
-        <v>1.72</v>
+        <f>980*10^-3</f>
+        <v>0.98</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>477.77777777777771</v>
+        <f>D6/C6</f>
+        <v>784</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3278,15 +5978,15 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C7">
-        <f>4.95*10^-3</f>
-        <v>4.9500000000000004E-3</v>
+        <f>1.95*10^-3</f>
+        <v>1.9499999999999999E-3</v>
       </c>
       <c r="D7">
-        <v>2.57</v>
+        <v>1.3</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>519.19191919191917</v>
+        <f t="shared" ref="E7:E13" si="0">D7/C7</f>
+        <v>666.66666666666674</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3298,15 +5998,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C8">
-        <f>5.2*10^-3</f>
-        <v>5.2000000000000006E-3</v>
+        <f>3.25*10^-3</f>
+        <v>3.2500000000000003E-3</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1.88</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>576.92307692307691</v>
+        <v>578.46153846153834</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3318,15 +6018,91 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C9">
-        <f>6.9*10^-3</f>
-        <v>6.9000000000000008E-3</v>
+        <f>3.95*10^-3</f>
+        <v>3.9500000000000004E-3</v>
       </c>
       <c r="D9">
-        <v>3.8</v>
+        <v>2.14</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>550.72463768115938</v>
+        <v>541.77215189873414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <f>5.55*10^-3</f>
+        <v>5.5500000000000002E-3</v>
+      </c>
+      <c r="D10">
+        <v>2.66</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>479.27927927927931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C11">
+        <f>6.2*10^-3</f>
+        <v>6.2000000000000006E-3</v>
+      </c>
+      <c r="D11">
+        <v>2.94</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>474.19354838709671</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C12">
+        <f>7.6*10^-3</f>
+        <v>7.6E-3</v>
+      </c>
+      <c r="D12">
+        <v>3.46</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>455.26315789473682</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.01</v>
+      </c>
+      <c r="C13">
+        <f>8.25*10^-3</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="D13">
+        <v>3.76</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>455.75757575757569</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -3363,16 +6139,16 @@
         <v>1E-3</v>
       </c>
       <c r="C20">
-        <f>1*10^-3</f>
-        <v>1E-3</v>
+        <f>(2.2*10^-3)/2</f>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="D20">
-        <f>1.32/2</f>
-        <v>0.66</v>
+        <f>(770*10^-3)/2</f>
+        <v>0.38500000000000001</v>
       </c>
       <c r="E20">
         <f>D20/C20</f>
-        <v>660</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,16 +6160,16 @@
         <v>2E-3</v>
       </c>
       <c r="C21">
-        <f>(3.95/2)*10^-3</f>
-        <v>1.9750000000000002E-3</v>
+        <f>(4*10^-3)/2</f>
+        <v>2E-3</v>
       </c>
       <c r="D21">
-        <f>2.58/2</f>
-        <v>1.29</v>
+        <f>1.54/2</f>
+        <v>0.77</v>
       </c>
       <c r="E21">
-        <f>D21/C21</f>
-        <v>653.16455696202524</v>
+        <f t="shared" ref="E21:E26" si="1">D21/C21</f>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3405,16 +6181,16 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C22">
-        <f>(6.05/2)*10^-3</f>
-        <v>3.0249999999999999E-3</v>
+        <f>(6.1*10^-3)/2</f>
+        <v>3.0499999999999998E-3</v>
       </c>
       <c r="D22">
-        <f>3.8/2</f>
-        <v>1.9</v>
+        <f>2.32/2</f>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E25" si="1">D22/C22</f>
-        <v>628.09917355371897</v>
+        <f t="shared" si="1"/>
+        <v>380.32786885245901</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3426,16 +6202,16 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C23">
-        <f>(8.25/2)*10^-3</f>
-        <v>4.1250000000000002E-3</v>
+        <f>(7.85*10^-3)/2</f>
+        <v>3.9249999999999997E-3</v>
       </c>
       <c r="D23">
-        <f>5.14/2</f>
-        <v>2.57</v>
+        <f>3.09/2</f>
+        <v>1.5449999999999999</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>623.030303030303</v>
+        <v>393.63057324840764</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,16 +6223,16 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C24">
-        <f>(10.1/2)*10^-3</f>
-        <v>5.0499999999999998E-3</v>
+        <f>(10.2*10^-3)/2</f>
+        <v>5.0999999999999995E-3</v>
       </c>
       <c r="D24">
-        <f>6.4/2</f>
-        <v>3.2</v>
+        <f>3.97/2</f>
+        <v>1.9850000000000001</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>633.66336633663377</v>
+        <v>389.21568627450984</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3468,16 +6244,96 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C25">
-        <f>6*10^-3</f>
-        <v>6.0000000000000001E-3</v>
+        <f>(12.2*10^-3)/2</f>
+        <v>6.0999999999999995E-3</v>
       </c>
       <c r="D25">
-        <f>7.6/2</f>
-        <v>3.8</v>
+        <f>4.74/2</f>
+        <v>2.37</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>633.33333333333326</v>
+        <v>388.52459016393448</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C26">
+        <f>(13.8*10^-3)/2</f>
+        <v>6.9000000000000008E-3</v>
+      </c>
+      <c r="D26">
+        <f>5.58/2</f>
+        <v>2.79</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>404.3478260869565</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C27">
+        <f>(15.9*10^-3)/2</f>
+        <v>7.9500000000000005E-3</v>
+      </c>
+      <c r="D27">
+        <f>6.44/2</f>
+        <v>3.22</v>
+      </c>
+      <c r="E27">
+        <f>D27/C27</f>
+        <v>405.03144654088049</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C28">
+        <f>(17.6*10^-3)/2</f>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D28">
+        <f>7.18/2</f>
+        <v>3.59</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28:E29" si="2">D28/C28</f>
+        <v>407.95454545454544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>0.01</v>
+      </c>
+      <c r="C29">
+        <f>(19.5*10^-3)/2</f>
+        <v>9.75E-3</v>
+      </c>
+      <c r="D29">
+        <f>7.96/2</f>
+        <v>3.98</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>408.20512820512818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Udregninger af fasedrej ved filter
</commit_message>
<xml_diff>
--- a/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
+++ b/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\Desktop\Semester-Projekt-3\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicoline\Desktop\Semester-Projekt-3\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark3" sheetId="3" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="Filter og forstærker sammen" sheetId="5" r:id="rId3"/>
     <sheet name="Forstærker" sheetId="1" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Forstærkning</t>
   </si>
@@ -155,9 +158,6 @@
     <t>Fasedrej</t>
   </si>
   <si>
-    <t>Amp i DB</t>
-  </si>
-  <si>
     <t>Integrationstest</t>
   </si>
   <si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Gain</t>
+  </si>
+  <si>
+    <t>Fasedrej i grader</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Filter!$A$3:$A$23</c:f>
+              <c:f>[1]Filter!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -457,7 +460,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Filter!$A$3:$A$23</c:f>
+              <c:f>[1]Filter!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -529,7 +532,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Filter!$C$3:$C$23</c:f>
+              <c:f>[1]Filter!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -609,8 +612,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343526552"/>
-        <c:axId val="343515576"/>
+        <c:axId val="470234576"/>
+        <c:axId val="470234968"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -644,7 +647,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Filter!$A$5:$A$22</c15:sqref>
+                          <c15:sqref>[1]Filter!$A$5:$A$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -713,7 +716,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Filter!$C$5:$C$22</c15:sqref>
+                          <c15:sqref>[1]Filter!$C$5:$C$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -784,7 +787,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343526552"/>
+        <c:axId val="470234576"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -842,12 +845,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343515576"/>
+        <c:crossAx val="470234968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343515576"/>
+        <c:axId val="470234968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,7 +907,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343526552"/>
+        <c:crossAx val="470234576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1031,7 +1034,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Filter!$A$27:$A$44</c:f>
+              <c:f>[1]Filter!$A$27:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1094,7 +1097,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Filter!$C$27:$C$44</c:f>
+              <c:f>[1]Filter!$C$27:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1165,8 +1168,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343516752"/>
-        <c:axId val="343517536"/>
+        <c:axId val="470214584"/>
+        <c:axId val="470210272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1200,7 +1203,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Filter!$A$27:$A$44</c15:sqref>
+                          <c15:sqref>[1]Filter!$A$27:$A$44</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1271,7 +1274,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343516752"/>
+        <c:axId val="470214584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1329,12 +1332,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343517536"/>
+        <c:crossAx val="470210272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343517536"/>
+        <c:axId val="470210272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,7 +1394,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343516752"/>
+        <c:crossAx val="470214584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1441,6 +1444,454 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fasedrejning</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> i grader</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6900481189851275E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.85721062992125985"/>
+          <c:h val="0.6714577865266842"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Serien</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Filter!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Filter!$E$3:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-16.559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-31.680000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-47.52000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-59.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-69.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-74.304000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-79.488</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-86.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-95.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-100.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-108</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-110.88000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-126.72000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-131.22</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-135</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-141.768</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-156.816</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-151.20000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="470213800"/>
+        <c:axId val="470218112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="470213800"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="500"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470218112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="470218112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470213800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
@@ -1714,11 +2165,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343517144"/>
-        <c:axId val="343514792"/>
+        <c:axId val="470390536"/>
+        <c:axId val="470397200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343517144"/>
+        <c:axId val="470390536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,12 +2226,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343514792"/>
+        <c:crossAx val="470397200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343514792"/>
+        <c:axId val="470397200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,7 +2288,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343517144"/>
+        <c:crossAx val="470390536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1886,7 +2337,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
@@ -2201,11 +2652,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343515184"/>
-        <c:axId val="343521848"/>
+        <c:axId val="470403080"/>
+        <c:axId val="470404256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343515184"/>
+        <c:axId val="470403080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2262,12 +2713,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343521848"/>
+        <c:crossAx val="470404256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343521848"/>
+        <c:axId val="470404256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2324,7 +2775,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343515184"/>
+        <c:crossAx val="470403080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2533,6 +2984,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4082,6 +4573,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4602,20 +5609,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagram 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="Diagram 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4633,19 +5642,21 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1285875</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagram 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Diagram 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4654,6 +5665,103 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Billede 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4362450" y="0"/>
+          <a:ext cx="1009650" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagram 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4725,6 +5833,401 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Ark3"/>
+      <sheetName val="Filter"/>
+      <sheetName val="Filter og forstærker sammen"/>
+      <sheetName val="Forstærker"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="A3">
+            <v>1</v>
+          </cell>
+          <cell r="C3">
+            <v>2.5</v>
+          </cell>
+          <cell r="E3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>5</v>
+          </cell>
+          <cell r="C4">
+            <v>2.5</v>
+          </cell>
+          <cell r="E4">
+            <v>-5.4</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>10</v>
+          </cell>
+          <cell r="C5">
+            <v>2.5</v>
+          </cell>
+          <cell r="E5">
+            <v>-16.559999999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>20</v>
+          </cell>
+          <cell r="C6">
+            <v>2.4700000000000002</v>
+          </cell>
+          <cell r="E6">
+            <v>-31.680000000000003</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>30</v>
+          </cell>
+          <cell r="C7">
+            <v>2.36</v>
+          </cell>
+          <cell r="E7">
+            <v>-47.52000000000001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>35</v>
+          </cell>
+          <cell r="C8">
+            <v>2.27</v>
+          </cell>
+          <cell r="E8">
+            <v>-59.22</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>40</v>
+          </cell>
+          <cell r="C9">
+            <v>2.14</v>
+          </cell>
+          <cell r="E9">
+            <v>-69.12</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>43</v>
+          </cell>
+          <cell r="C10">
+            <v>2.04</v>
+          </cell>
+          <cell r="E10">
+            <v>-74.304000000000002</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>46</v>
+          </cell>
+          <cell r="C11">
+            <v>1.97</v>
+          </cell>
+          <cell r="E11">
+            <v>-79.488</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>50</v>
+          </cell>
+          <cell r="C12">
+            <v>1.81</v>
+          </cell>
+          <cell r="E12">
+            <v>-86.4</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>53</v>
+          </cell>
+          <cell r="C13">
+            <v>1.72</v>
+          </cell>
+          <cell r="E13">
+            <v>-95.4</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>56</v>
+          </cell>
+          <cell r="C14">
+            <v>1.61</v>
+          </cell>
+          <cell r="E14">
+            <v>-100.8</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>60</v>
+          </cell>
+          <cell r="C15">
+            <v>1.48</v>
+          </cell>
+          <cell r="E15">
+            <v>-108</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>70</v>
+          </cell>
+          <cell r="C16">
+            <v>1.18</v>
+          </cell>
+          <cell r="E16">
+            <v>-110.88000000000002</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>80</v>
+          </cell>
+          <cell r="C17">
+            <v>0.96</v>
+          </cell>
+          <cell r="E17">
+            <v>-126.72000000000001</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>90</v>
+          </cell>
+          <cell r="C18">
+            <v>0.77</v>
+          </cell>
+          <cell r="E18">
+            <v>-131.22</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>100</v>
+          </cell>
+          <cell r="C19">
+            <v>0.64</v>
+          </cell>
+          <cell r="E19">
+            <v>-135</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>110</v>
+          </cell>
+          <cell r="C20">
+            <v>0.55000000000000004</v>
+          </cell>
+          <cell r="E20">
+            <v>-141.768</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>120</v>
+          </cell>
+          <cell r="C21">
+            <v>0.46</v>
+          </cell>
+          <cell r="E21">
+            <v>-156.816</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>150</v>
+          </cell>
+          <cell r="C22">
+            <v>0.28999999999999998</v>
+          </cell>
+          <cell r="E22">
+            <v>-151.20000000000002</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>500</v>
+          </cell>
+          <cell r="C23">
+            <v>2.75E-2</v>
+          </cell>
+          <cell r="E23">
+            <v>-180</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>10</v>
+          </cell>
+          <cell r="C27">
+            <v>7.9588001734407516</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>20</v>
+          </cell>
+          <cell r="C28">
+            <v>7.8539390651933152</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>30</v>
+          </cell>
+          <cell r="C29">
+            <v>7.4582400594021312</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>35</v>
+          </cell>
+          <cell r="C30">
+            <v>7.1205171438624548</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>40</v>
+          </cell>
+          <cell r="C31">
+            <v>6.6082754669838177</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>43</v>
+          </cell>
+          <cell r="C32">
+            <v>6.1926033485179754</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>46</v>
+          </cell>
+          <cell r="C33">
+            <v>5.8893245232318581</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>50</v>
+          </cell>
+          <cell r="C34">
+            <v>5.1535714973836901</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>53</v>
+          </cell>
+          <cell r="C35">
+            <v>4.7105689381509777</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>56</v>
+          </cell>
+          <cell r="C36">
+            <v>4.1365175206369944</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>60</v>
+          </cell>
+          <cell r="C37">
+            <v>3.4052343078991476</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>70</v>
+          </cell>
+          <cell r="C38">
+            <v>1.4376401461225072</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>80</v>
+          </cell>
+          <cell r="C39">
+            <v>-0.35457533920863205</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>90</v>
+          </cell>
+          <cell r="C40">
+            <v>-2.2701854965503623</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>100</v>
+          </cell>
+          <cell r="C41">
+            <v>-3.8764005203222562</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>110</v>
+          </cell>
+          <cell r="C42">
+            <v>-5.1927462101151223</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>120</v>
+          </cell>
+          <cell r="C43">
+            <v>-6.7448433663685181</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>150</v>
+          </cell>
+          <cell r="C44">
+            <v>-10.752040042020878</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5301,8 +6804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5310,6 +6813,7 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5326,7 +6830,7 @@
         <v>38</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5342,6 +6846,10 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3">
+        <f>360*A3*D3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -5356,6 +6864,10 @@
       <c r="D4">
         <v>3</v>
       </c>
+      <c r="E4">
+        <f>-360*A4*D4*10^-3</f>
+        <v>-5.4</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -5370,6 +6882,10 @@
       <c r="D5">
         <v>4.5999999999999996</v>
       </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E22" si="0">-360*A5*D5*10^-3</f>
+        <v>-16.559999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -5385,6 +6901,10 @@
       <c r="D6">
         <v>4.4000000000000004</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-31.680000000000003</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -5400,6 +6920,10 @@
       <c r="D7">
         <v>4.4000000000000004</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-47.52000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -5415,6 +6939,10 @@
       <c r="D8">
         <v>4.7</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-59.22</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -5430,6 +6958,10 @@
       <c r="D9">
         <v>4.8</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-69.12</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -5445,6 +6977,10 @@
       <c r="D10">
         <v>4.8</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-74.304000000000002</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -5460,6 +6996,10 @@
       <c r="D11">
         <v>4.8</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-79.488</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -5475,6 +7015,10 @@
       <c r="D12">
         <v>4.8</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-86.4</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -5490,6 +7034,10 @@
       <c r="D13">
         <v>5</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-95.4</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -5505,6 +7053,10 @@
       <c r="D14">
         <v>5</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-100.8</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -5520,6 +7072,10 @@
       <c r="D15">
         <v>5</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>-108</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -5535,8 +7091,12 @@
       <c r="D16">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-110.88000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>80</v>
       </c>
@@ -5550,8 +7110,12 @@
       <c r="D17">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-126.72000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>90</v>
       </c>
@@ -5565,8 +7129,12 @@
       <c r="D18">
         <v>4.05</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>-131.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>100</v>
       </c>
@@ -5580,8 +7148,12 @@
       <c r="D19">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>110</v>
       </c>
@@ -5595,8 +7167,12 @@
       <c r="D20">
         <v>3.58</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-141.768</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>120</v>
       </c>
@@ -5610,8 +7186,12 @@
       <c r="D21">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>-156.816</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>150</v>
       </c>
@@ -5625,8 +7205,12 @@
       <c r="D22">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>-151.20000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>500</v>
       </c>
@@ -5640,19 +7224,19 @@
       <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -5664,7 +7248,7 @@
         <v>7.9588001734407516</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -5673,11 +7257,11 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:C44" si="0">20*LOG10(B28)</f>
+        <f t="shared" ref="C28:C44" si="1">20*LOG10(B28)</f>
         <v>7.8539390651933152</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>30</v>
       </c>
@@ -5686,11 +7270,11 @@
         <v>2.36</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4582400594021312</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>35</v>
       </c>
@@ -5699,11 +7283,11 @@
         <v>2.27</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1205171438624548</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>40</v>
       </c>
@@ -5712,11 +7296,11 @@
         <v>2.14</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6082754669838177</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>43</v>
       </c>
@@ -5725,7 +7309,7 @@
         <v>2.04</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.1926033485179754</v>
       </c>
     </row>
@@ -5738,7 +7322,7 @@
         <v>1.97</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8893245232318581</v>
       </c>
     </row>
@@ -5751,7 +7335,7 @@
         <v>1.81</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1535714973836901</v>
       </c>
     </row>
@@ -5764,7 +7348,7 @@
         <v>1.72</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7105689381509777</v>
       </c>
     </row>
@@ -5777,7 +7361,7 @@
         <v>1.61</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1365175206369944</v>
       </c>
     </row>
@@ -5790,7 +7374,7 @@
         <v>1.48</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4052343078991476</v>
       </c>
     </row>
@@ -5803,7 +7387,7 @@
         <v>1.18</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4376401461225072</v>
       </c>
     </row>
@@ -5816,7 +7400,7 @@
         <v>0.96</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.35457533920863205</v>
       </c>
     </row>
@@ -5829,7 +7413,7 @@
         <v>0.77</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.2701854965503623</v>
       </c>
     </row>
@@ -5842,7 +7426,7 @@
         <v>0.64</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.8764005203222562</v>
       </c>
     </row>
@@ -5855,7 +7439,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.1927462101151223</v>
       </c>
     </row>
@@ -5868,7 +7452,7 @@
         <v>0.46</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.7448433663685181</v>
       </c>
     </row>
@@ -5881,7 +7465,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-10.752040042020878</v>
       </c>
     </row>
@@ -5896,7 +7480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -5913,7 +7497,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -5921,19 +7505,19 @@
         <v>37</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>41</v>
@@ -6234,7 +7818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Logbog og måledata opdateret
</commit_message>
<xml_diff>
--- a/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
+++ b/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ark3" sheetId="3" r:id="rId1"/>
     <sheet name="Filter" sheetId="4" r:id="rId2"/>
-    <sheet name="Filter og forstærker sammen" sheetId="5" r:id="rId3"/>
-    <sheet name="Forstærker" sheetId="1" r:id="rId4"/>
+    <sheet name="Vandsøjle" sheetId="6" r:id="rId3"/>
+    <sheet name="Filter og forstærker sammen" sheetId="5" r:id="rId4"/>
+    <sheet name="Forstærker" sheetId="1" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Forstærkning</t>
   </si>
@@ -174,6 +175,18 @@
   </si>
   <si>
     <t>Fasedrej i grader</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>Vandsøjle i mm</t>
+  </si>
+  <si>
+    <t>Målt input i V</t>
+  </si>
+  <si>
+    <t>Output i V</t>
   </si>
 </sst>
 </file>
@@ -369,69 +382,9 @@
             <c:strRef>
               <c:f>[1]Filter!$A$3:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>500</c:v>
+                  <c:v>1 5 10 20 30 35 40 43 46 50 53 56 60 70 80 90 100 110 120 150 500</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -612,8 +565,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="470234576"/>
-        <c:axId val="470234968"/>
+        <c:axId val="412177272"/>
+        <c:axId val="412178840"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -787,7 +740,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="470234576"/>
+        <c:axId val="412177272"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -845,12 +798,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470234968"/>
+        <c:crossAx val="412178840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="470234968"/>
+        <c:axId val="412178840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +860,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470234576"/>
+        <c:crossAx val="412177272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -971,7 +924,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1168,8 +1120,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="470214584"/>
-        <c:axId val="470210272"/>
+        <c:axId val="412174920"/>
+        <c:axId val="412180016"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1274,7 +1226,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="470214584"/>
+        <c:axId val="412174920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1332,12 +1284,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470210272"/>
+        <c:crossAx val="412180016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="470210272"/>
+        <c:axId val="412180016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1346,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470214584"/>
+        <c:crossAx val="412174920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1716,11 +1668,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="470213800"/>
-        <c:axId val="470218112"/>
+        <c:axId val="412168648"/>
+        <c:axId val="412169824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="470213800"/>
+        <c:axId val="412168648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1780,12 +1732,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470218112"/>
+        <c:crossAx val="412169824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="470218112"/>
+        <c:axId val="412169824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1842,7 +1794,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470213800"/>
+        <c:crossAx val="412168648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2165,11 +2117,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="470390536"/>
-        <c:axId val="470397200"/>
+        <c:axId val="412170608"/>
+        <c:axId val="412171000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="470390536"/>
+        <c:axId val="412170608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,12 +2178,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470397200"/>
+        <c:crossAx val="412171000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="470397200"/>
+        <c:axId val="412171000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2288,7 +2240,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470390536"/>
+        <c:crossAx val="412170608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2652,11 +2604,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="470403080"/>
-        <c:axId val="470404256"/>
+        <c:axId val="415839880"/>
+        <c:axId val="415843408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="470403080"/>
+        <c:axId val="415839880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2713,12 +2665,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470404256"/>
+        <c:crossAx val="415843408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="470404256"/>
+        <c:axId val="415843408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2775,7 +2727,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470403080"/>
+        <c:crossAx val="415839880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6804,7 +6756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -7477,6 +7429,90 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>1360</v>
+      </c>
+      <c r="D2">
+        <f>2.1*10^-3</f>
+        <v>2.1000000000000003E-3</v>
+      </c>
+      <c r="E2">
+        <f>945*10^-3</f>
+        <v>0.94500000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>680</v>
+      </c>
+      <c r="D3">
+        <f>-261*10^-3</f>
+        <v>-0.26100000000000001</v>
+      </c>
+      <c r="E3">
+        <f>-8*10^-3</f>
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>136</v>
+      </c>
+      <c r="D4">
+        <f>-1.8*10^-3</f>
+        <v>-1.8000000000000002E-3</v>
+      </c>
+      <c r="E4">
+        <f>-24.2*10^-3</f>
+        <v>-2.4199999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H36"/>
   <sheetViews>
@@ -7814,11 +7850,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Logbog, test og beregninger
</commit_message>
<xml_diff>
--- a/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
+++ b/Hardware/TheGoldenDoc (reg af forstærker) & filter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark3" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Forstærkning</t>
   </si>
@@ -188,6 +188,15 @@
   <si>
     <t>Output i V</t>
   </si>
+  <si>
+    <t>Logartmisk skala (amplitude værdier i dB)</t>
+  </si>
+  <si>
+    <t>Frekvens i Hz</t>
+  </si>
+  <si>
+    <t>Oprindelig input</t>
+  </si>
 </sst>
 </file>
 
@@ -225,12 +234,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -265,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -277,6 +298,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,8 +588,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412177272"/>
-        <c:axId val="412178840"/>
+        <c:axId val="386455736"/>
+        <c:axId val="386456128"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -740,7 +763,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412177272"/>
+        <c:axId val="386455736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -798,12 +821,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412178840"/>
+        <c:crossAx val="386456128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412178840"/>
+        <c:axId val="386456128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,7 +883,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412177272"/>
+        <c:crossAx val="386455736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -924,6 +947,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="da-DK"/>
+              <a:t>Amplitude</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" baseline="0"/>
+              <a:t> i dB (y), frekvenser i log på x akse</a:t>
+            </a:r>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1120,8 +1174,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412174920"/>
-        <c:axId val="412180016"/>
+        <c:axId val="386456520"/>
+        <c:axId val="386457304"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1226,7 +1280,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412174920"/>
+        <c:axId val="386456520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1284,12 +1338,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412180016"/>
+        <c:crossAx val="386457304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412180016"/>
+        <c:axId val="386457304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1346,7 +1400,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412174920"/>
+        <c:crossAx val="386456520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1668,11 +1722,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412168648"/>
-        <c:axId val="412169824"/>
+        <c:axId val="386458480"/>
+        <c:axId val="386460048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412168648"/>
+        <c:axId val="386458480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1713,7 +1767,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1732,12 +1786,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412169824"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="386460048"/>
+        <c:crossesAt val="-200"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412169824"/>
+        <c:axId val="386460048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1848,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412168648"/>
+        <c:crossAx val="386458480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1844,6 +1898,1113 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lav amplitude</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$B$5,'Filter og forstærker sammen'!$B$7,'Filter og forstærker sammen'!$B$9,'Filter og forstærker sammen'!$B$11,'Filter og forstærker sammen'!$B$13,'Filter og forstærker sammen'!$B$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$E$4,'Filter og forstærker sammen'!$E$6,'Filter og forstærker sammen'!$E$8,'Filter og forstærker sammen'!$E$10,'Filter og forstærker sammen'!$E$12,'Filter og forstærker sammen'!$E$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.689075023018618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1499207582642583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5750720190565781</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7609220625759079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8066339634058299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9843822531075976</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Høj amplitude</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$B$5,'Filter og forstærker sammen'!$B$7,'Filter og forstærker sammen'!$B$9,'Filter og forstærker sammen'!$B$11,'Filter og forstærker sammen'!$B$13,'Filter og forstærker sammen'!$B$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$E$5,'Filter og forstærker sammen'!$E$7,'Filter og forstærker sammen'!$E$9,'Filter og forstærker sammen'!$E$11,'Filter og forstærker sammen'!$E$13,'Filter og forstærker sammen'!$E$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.2994669594163604</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4949669202020779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8878454737022139</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.107027388932476</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2014277597014953</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2968769609539574</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="504323808"/>
+        <c:axId val="504325376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="504323808"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504325376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="504325376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504323808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lav amplitude</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.42185192475940508"/>
+                  <c:y val="0.31746609798775155"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>y = -0,0306x + 3,2515</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>R² = 0,9963</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$B$5,'Filter og forstærker sammen'!$B$7,'Filter og forstærker sammen'!$B$9,'Filter og forstærker sammen'!$B$11,'Filter og forstærker sammen'!$B$13,'Filter og forstærker sammen'!$B$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$D$4,'Filter og forstærker sammen'!$D$6,'Filter og forstærker sammen'!$D$8,'Filter og forstærker sammen'!$D$10,'Filter og forstærker sammen'!$D$12,'Filter og forstærker sammen'!$D$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Høj amplitude</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.44129636920384951"/>
+                  <c:y val="-0.16457531350247886"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent4"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>y = -0,0379x + 3,9123</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent4"/>
+                        </a:solidFill>
+                      </a:rPr>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent4"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>R² = 0,9985</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$B$5,'Filter og forstærker sammen'!$B$7,'Filter og forstærker sammen'!$B$9,'Filter og forstærker sammen'!$B$11,'Filter og forstærker sammen'!$B$13,'Filter og forstærker sammen'!$B$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Filter og forstærker sammen'!$D$5,'Filter og forstærker sammen'!$D$7,'Filter og forstærker sammen'!$D$9,'Filter og forstærker sammen'!$D$11,'Filter og forstærker sammen'!$D$13,'Filter og forstærker sammen'!$D$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="392141552"/>
+        <c:axId val="392132536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="392141552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392132536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="392132536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392141552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
@@ -2117,11 +3278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412170608"/>
-        <c:axId val="412171000"/>
+        <c:axId val="389224064"/>
+        <c:axId val="389219360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412170608"/>
+        <c:axId val="389224064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,12 +3339,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412171000"/>
+        <c:crossAx val="389219360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412171000"/>
+        <c:axId val="389219360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,7 +3401,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412170608"/>
+        <c:crossAx val="389224064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2289,7 +3450,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
@@ -2604,11 +3765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="415839880"/>
-        <c:axId val="415843408"/>
+        <c:axId val="389217400"/>
+        <c:axId val="389214656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="415839880"/>
+        <c:axId val="389217400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2665,12 +3826,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415843408"/>
+        <c:crossAx val="389214656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="415843408"/>
+        <c:axId val="389214656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2727,7 +3888,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415839880"/>
+        <c:crossAx val="389217400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2976,6 +4137,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5041,6 +6282,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5563,13 +7836,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>185738</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5726,16 +7999,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5756,16 +8029,148 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Billede 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8191500" y="190500"/>
+          <a:ext cx="1009650" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6756,8 +9161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7187,6 +9592,9 @@
       <c r="B26" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -7430,10 +9838,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7443,9 +9851,10 @@
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -7458,8 +9867,11 @@
       <c r="E1" t="s">
         <v>51</v>
       </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -7474,8 +9886,12 @@
         <f>945*10^-3</f>
         <v>0.94500000000000006</v>
       </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F3" si="0">E2/D2</f>
+        <v>449.99999999999994</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -7483,15 +9899,18 @@
         <v>680</v>
       </c>
       <c r="D3">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="E3">
         <f>-261*10^-3</f>
         <v>-0.26100000000000001</v>
       </c>
-      <c r="E3">
-        <f>-8*10^-3</f>
-        <v>-8.0000000000000002E-3</v>
+      <c r="F3">
+        <f>E3/D3</f>
+        <v>32.625</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7505,6 +9924,10 @@
       <c r="E4">
         <f>-24.2*10^-3</f>
         <v>-2.4199999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <f>E4/D4</f>
+        <v>13.444444444444443</v>
       </c>
     </row>
   </sheetData>
@@ -7516,8 +9939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7538,7 +9961,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>43</v>
@@ -7560,25 +9983,29 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="7">
         <v>35</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>2.16</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <f>20*LOG10(D4)</f>
         <v>6.689075023018618</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <f>D4/C4</f>
         <v>360</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>4.8</v>
+      </c>
+      <c r="H4" s="7">
+        <f>-360*B4*G4*10^-3</f>
+        <v>-60.480000000000004</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -7602,27 +10029,35 @@
       <c r="G5">
         <v>4.8</v>
       </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:H15" si="2">-360*B5*G5*10^-3</f>
+        <v>-60.480000000000004</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="7">
         <v>40</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="7">
         <f t="shared" si="0"/>
         <v>6.1499207582642583</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7">
         <f t="shared" si="1"/>
         <v>338.33333333333331</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="7">
         <v>4.5</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="2"/>
+        <v>-64.8</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -7646,27 +10081,35 @@
       <c r="G7">
         <v>4.5</v>
       </c>
+      <c r="H7" s="8">
+        <f t="shared" si="2"/>
+        <v>-64.8</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="7">
         <v>45</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <v>1.9</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="7">
         <f t="shared" si="0"/>
         <v>5.5750720190565781</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <f t="shared" si="1"/>
         <v>316.66666666666663</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="7">
         <v>4.7</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="2"/>
+        <v>-76.14</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -7690,27 +10133,35 @@
       <c r="G9">
         <v>4.7</v>
       </c>
+      <c r="H9" s="8">
+        <f t="shared" si="2"/>
+        <v>-76.14</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="7">
         <v>50</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <v>1.73</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7">
         <f t="shared" si="0"/>
         <v>4.7609220625759079</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="7">
         <f t="shared" si="1"/>
         <v>288.33333333333331</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7">
         <v>4.4000000000000004</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="2"/>
+        <v>-79.2</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -7734,27 +10185,35 @@
       <c r="G11">
         <v>4.4000000000000004</v>
       </c>
+      <c r="H11" s="8">
+        <f t="shared" si="2"/>
+        <v>-79.2</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="7">
         <v>55</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>1.55</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7">
         <f t="shared" si="0"/>
         <v>3.8066339634058299</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <f t="shared" si="1"/>
         <v>258.33333333333331</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="7">
         <v>4.7</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="2"/>
+        <v>-93.06</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -7778,27 +10237,35 @@
       <c r="G13">
         <v>4.7</v>
       </c>
+      <c r="H13" s="8">
+        <f t="shared" si="2"/>
+        <v>-93.06</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="7">
         <v>60</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="7">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>1.41</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <f t="shared" si="0"/>
         <v>2.9843822531075976</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <f t="shared" si="1"/>
         <v>234.99999999999997</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>4.4000000000000004</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="2"/>
+        <v>-95.04000000000002</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -7821,6 +10288,10 @@
       </c>
       <c r="G15">
         <v>4.4000000000000004</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="2"/>
+        <v>-95.04000000000002</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -7847,15 +10318,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E29"/>
+  <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7865,14 +10337,16 @@
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7889,7 +10363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7901,7 +10375,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -7912,8 +10386,14 @@
       <c r="C5" t="s">
         <v>40</v>
       </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -7933,8 +10413,16 @@
         <f>D6/C6</f>
         <v>784</v>
       </c>
+      <c r="F6">
+        <f>C6+0.0012</f>
+        <v>2.4499999999999999E-3</v>
+      </c>
+      <c r="G6">
+        <f>D6/F6</f>
+        <v>400</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -7953,8 +10441,16 @@
         <f t="shared" ref="E7:E13" si="0">D7/C7</f>
         <v>666.66666666666674</v>
       </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F13" si="1">C7+0.0012</f>
+        <v>3.15E-3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G13" si="2">D7/F7</f>
+        <v>412.69841269841271</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -7973,8 +10469,16 @@
         <f t="shared" si="0"/>
         <v>578.46153846153834</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4.45E-3</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>422.47191011235952</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -7993,8 +10497,16 @@
         <f t="shared" si="0"/>
         <v>541.77215189873414</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>5.1500000000000001E-3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>415.53398058252429</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -8012,8 +10524,16 @@
         <f t="shared" si="0"/>
         <v>479.27927927927931</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>6.7499999999999999E-3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>394.07407407407408</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -8031,8 +10551,16 @@
         <f t="shared" si="0"/>
         <v>474.19354838709671</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>397.29729729729729</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -8050,8 +10578,16 @@
         <f t="shared" si="0"/>
         <v>455.26315789473682</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>393.18181818181813</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -8069,8 +10605,16 @@
         <f t="shared" si="0"/>
         <v>455.75757575757569</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>9.4500000000000001E-3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>397.88359788359787</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
@@ -8078,7 +10622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -8095,7 +10639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -8115,8 +10659,16 @@
         <f>D20/C20</f>
         <v>350</v>
       </c>
+      <c r="F20">
+        <f>C20-0.1375*10^-3</f>
+        <v>9.6250000000000003E-4</v>
+      </c>
+      <c r="G20">
+        <f>D20/F20</f>
+        <v>400</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -8133,11 +10685,19 @@
         <v>0.77</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E26" si="1">D21/C21</f>
+        <f t="shared" ref="E21:E26" si="3">D21/C21</f>
         <v>385</v>
       </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F29" si="4">C21-0.1375*10^-3</f>
+        <v>1.8625E-3</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G29" si="5">D21/F21</f>
+        <v>413.42281879194633</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -8154,11 +10714,19 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>380.32786885245901</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>2.9124999999999997E-3</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>398.28326180257511</v>
+      </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -8175,11 +10743,19 @@
         <v>1.5449999999999999</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>393.63057324840764</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>3.7874999999999996E-3</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>407.92079207920796</v>
+      </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -8196,11 +10772,19 @@
         <v>1.9850000000000001</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>389.21568627450984</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>4.9624999999999999E-3</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>400</v>
+      </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -8217,11 +10801,19 @@
         <v>2.37</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>388.52459016393448</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>5.9624999999999999E-3</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>397.48427672955978</v>
+      </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -8237,11 +10829,19 @@
         <v>2.79</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>404.3478260869565</v>
       </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>6.7625000000000011E-3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>412.56931608133078</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -8260,8 +10860,16 @@
         <f>D27/C27</f>
         <v>405.03144654088049</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>412.16</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -8277,11 +10885,19 @@
         <v>3.59</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E29" si="2">D28/C28</f>
+        <f t="shared" ref="E28:E29" si="6">D28/C28</f>
         <v>407.95454545454544</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>8.6625000000000001E-3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>414.43001443001441</v>
+      </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -8297,8 +10913,16 @@
         <v>3.98</v>
       </c>
       <c r="E29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>408.20512820512818</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>9.6124999999999995E-3</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>414.0442132639792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>